<commit_message>
PROS-7786 - CCRU - KPI Calculation fix
</commit_message>
<xml_diff>
--- a/Projects/CCRU/Data/KPIs_2019/PoS 2019 - MT Conv Big - REG.xlsx
+++ b/Projects/CCRU/Data/KPIs_2019/PoS 2019 - MT Conv Big - REG.xlsx
@@ -15,6 +15,7 @@
     <definedName function="false" hidden="false" localSheetId="0" name="_FilterDatabase_0" vbProcedure="false">CONV_BIG_REG!$A$1:$AP$178</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">CONV_BIG_REG!$A$1:$AP$178</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0" vbProcedure="false">CONV_BIG_REG!$A$1:$AP$178</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">CONV_BIG_REG!$A$1:$AP$178</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -2337,51 +2338,51 @@
   <dimension ref="A1:AP178"/>
   <sheetViews>
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A138" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A89" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A154" activeCellId="0" sqref="A154"/>
+      <selection pane="bottomLeft" activeCell="A117" activeCellId="0" sqref="A117"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="10.1781376518219"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="10.2834008097166"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="1" width="11.0323886639676"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="17.8906882591093"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="17.995951417004"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="1" width="10.9271255060729"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="15.1052631578947"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="47.3481781376518"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="65.2348178137652"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="47.1336032388664"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="16.1740890688259"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="15.2105263157895"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="47.7732793522267"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="65.7692307692308"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="47.4534412955466"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="16.2834008097166"/>
     <col collapsed="false" hidden="false" max="10" min="10" style="2" width="9"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="3" width="13.2834008097166"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="3" width="13.3886639676113"/>
     <col collapsed="false" hidden="false" max="12" min="12" style="3" width="13.497975708502"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="43.0607287449393"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="30.5303643724696"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="19.7085020242915"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="1" width="15.8542510121457"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="43.4898785425101"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="30.7449392712551"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="19.8178137651822"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="1" width="15.9595141700405"/>
     <col collapsed="false" hidden="false" max="17" min="17" style="1" width="9.10526315789474"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="1" width="18.5303643724696"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="1" width="18.6396761133603"/>
     <col collapsed="false" hidden="false" max="19" min="19" style="1" width="13.3886639676113"/>
     <col collapsed="false" hidden="false" max="20" min="20" style="1" width="6.96356275303644"/>
     <col collapsed="false" hidden="false" max="21" min="21" style="1" width="13.9271255060729"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="1" width="80.9838056680162"/>
-    <col collapsed="false" hidden="false" max="23" min="23" style="1" width="22.3886639676113"/>
-    <col collapsed="false" hidden="false" max="24" min="24" style="1" width="46.4898785425101"/>
-    <col collapsed="false" hidden="false" max="25" min="25" style="1" width="52.165991902834"/>
-    <col collapsed="false" hidden="false" max="26" min="26" style="1" width="19.9230769230769"/>
-    <col collapsed="false" hidden="false" max="27" min="27" style="1" width="25.2793522267206"/>
-    <col collapsed="false" hidden="false" max="28" min="28" style="1" width="25.7085020242915"/>
-    <col collapsed="false" hidden="false" max="29" min="29" style="1" width="15.5303643724696"/>
+    <col collapsed="false" hidden="false" max="22" min="22" style="1" width="81.7327935222672"/>
+    <col collapsed="false" hidden="false" max="23" min="23" style="1" width="22.4939271255061"/>
+    <col collapsed="false" hidden="false" max="24" min="24" style="1" width="46.8097165991903"/>
+    <col collapsed="false" hidden="false" max="25" min="25" style="1" width="52.5951417004049"/>
+    <col collapsed="false" hidden="false" max="26" min="26" style="1" width="20.0323886639676"/>
+    <col collapsed="false" hidden="false" max="27" min="27" style="1" width="25.4939271255061"/>
+    <col collapsed="false" hidden="false" max="28" min="28" style="1" width="25.8137651821862"/>
+    <col collapsed="false" hidden="false" max="29" min="29" style="1" width="15.6396761133603"/>
     <col collapsed="false" hidden="false" max="30" min="30" style="1" width="13.6032388663968"/>
-    <col collapsed="false" hidden="false" max="31" min="31" style="1" width="25.7085020242915"/>
+    <col collapsed="false" hidden="false" max="31" min="31" style="1" width="25.8137651821862"/>
     <col collapsed="false" hidden="false" max="32" min="32" style="1" width="13.9271255060729"/>
-    <col collapsed="false" hidden="false" max="33" min="33" style="1" width="12.5344129554656"/>
-    <col collapsed="false" hidden="false" max="34" min="34" style="1" width="13.0688259109312"/>
-    <col collapsed="false" hidden="false" max="35" min="35" style="1" width="60.5222672064777"/>
-    <col collapsed="false" hidden="false" max="36" min="36" style="1" width="25.7085020242915"/>
-    <col collapsed="false" hidden="false" max="37" min="37" style="1" width="20.5668016194332"/>
-    <col collapsed="false" hidden="false" max="38" min="38" style="1" width="21.7449392712551"/>
+    <col collapsed="false" hidden="false" max="33" min="33" style="1" width="12.6396761133603"/>
+    <col collapsed="false" hidden="false" max="34" min="34" style="1" width="13.1740890688259"/>
+    <col collapsed="false" hidden="false" max="35" min="35" style="1" width="61.0566801619433"/>
+    <col collapsed="false" hidden="false" max="36" min="36" style="1" width="25.8137651821862"/>
+    <col collapsed="false" hidden="false" max="37" min="37" style="1" width="20.6720647773279"/>
+    <col collapsed="false" hidden="false" max="38" min="38" style="1" width="21.9595141700405"/>
     <col collapsed="false" hidden="false" max="39" min="39" style="1" width="7.60728744939271"/>
     <col collapsed="false" hidden="false" max="40" min="40" style="1" width="8.67611336032389"/>
     <col collapsed="false" hidden="false" max="41" min="41" style="1" width="10.6032388663968"/>
@@ -11856,7 +11857,7 @@
       <c r="Y114" s="12"/>
       <c r="Z114" s="12"/>
       <c r="AA114" s="15" t="n">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="AB114" s="12"/>
       <c r="AC114" s="12"/>
@@ -11944,7 +11945,7 @@
       <c r="Y115" s="12"/>
       <c r="Z115" s="12"/>
       <c r="AA115" s="15" t="n">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="AB115" s="12"/>
       <c r="AC115" s="12"/>
@@ -12024,7 +12025,7 @@
       <c r="Y116" s="12"/>
       <c r="Z116" s="12"/>
       <c r="AA116" s="15" t="n">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="AB116" s="12"/>
       <c r="AC116" s="12"/>
@@ -12106,7 +12107,7 @@
       <c r="Y117" s="12"/>
       <c r="Z117" s="12"/>
       <c r="AA117" s="15" t="n">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="AB117" s="12"/>
       <c r="AC117" s="12"/>

</xml_diff>

<commit_message>
PROS-8045 - BATRU - Additional filers and POSM in API
</commit_message>
<xml_diff>
--- a/Projects/CCRU/Data/KPIs_2019/PoS 2019 - MT Conv Big - REG.xlsx
+++ b/Projects/CCRU/Data/KPIs_2019/PoS 2019 - MT Conv Big - REG.xlsx
@@ -16,6 +16,7 @@
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0" vbProcedure="false">CONV_BIG_REG!$A$1:$AQ$181</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">CONV_BIG_REG!$A$1:$AQ$181</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">CONV_BIG_REG!$A$1:$AQ$181</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">CONV_BIG_REG!$A$1:$AQ$181</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2430" uniqueCount="597">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2430" uniqueCount="596">
   <si>
     <t xml:space="preserve">Sorting</t>
   </si>
@@ -1809,9 +1810,6 @@
   </si>
   <si>
     <t xml:space="preserve">Dobriy 0.33 in Bakery</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dobriy 0.33 in Bakery </t>
   </si>
   <si>
     <t xml:space="preserve">Hidden</t>
@@ -2407,53 +2405,53 @@
   </sheetPr>
   <dimension ref="1:182"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="AC1" colorId="64" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A164" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="AC1" activeCellId="0" sqref="AC1"/>
-      <selection pane="bottomLeft" activeCell="AP172" activeCellId="0" sqref="AP172"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="A167" activeCellId="0" sqref="A167"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="22.45"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="10.0688259109312"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="10.1781376518219"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="1" width="11.0323886639676"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="17.7813765182186"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="17.8906882591093"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="1" width="10.9271255060729"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="14.8906882591093"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="41.3481781376518"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="46.8097165991903"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="64.165991902834"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="46.3805668016194"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="16.0688259109312"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="14.9959514170041"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="41.668016194332"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="47.1336032388664"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="64.7004048582996"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="46.7044534412956"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="16.1740890688259"/>
     <col collapsed="false" hidden="false" max="11" min="11" style="1" width="9"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="13.1740890688259"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="13.2834008097166"/>
     <col collapsed="false" hidden="false" max="13" min="13" style="1" width="13.497975708502"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="55.5951417004049"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="30.1012145748988"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="1" width="19.3886639676113"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="1" width="15.7449392712551"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="56.0242914979757"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="30.3157894736842"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="1" width="19.4939271255061"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="1" width="15.8542510121457"/>
     <col collapsed="false" hidden="false" max="18" min="18" style="1" width="9.10526315789474"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="1" width="18.4251012145749"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="1" width="18.5303643724696"/>
     <col collapsed="false" hidden="false" max="20" min="20" style="1" width="13.3886639676113"/>
     <col collapsed="false" hidden="false" max="21" min="21" style="1" width="6.96356275303644"/>
     <col collapsed="false" hidden="false" max="22" min="22" style="1" width="13.9271255060729"/>
-    <col collapsed="false" hidden="false" max="23" min="23" style="1" width="79.6963562753036"/>
-    <col collapsed="false" hidden="false" max="24" min="24" style="1" width="22.0647773279352"/>
-    <col collapsed="false" hidden="false" max="25" min="25" style="1" width="116.117408906883"/>
-    <col collapsed="false" hidden="false" max="26" min="26" style="1" width="51.3117408906883"/>
-    <col collapsed="false" hidden="false" max="27" min="27" style="1" width="19.6032388663968"/>
-    <col collapsed="false" hidden="false" max="28" min="28" style="1" width="24.8502024291498"/>
-    <col collapsed="false" hidden="false" max="29" min="29" style="1" width="25.3886639676113"/>
-    <col collapsed="false" hidden="false" max="30" min="30" style="1" width="15.4251012145749"/>
+    <col collapsed="false" hidden="false" max="23" min="23" style="1" width="80.3400809716599"/>
+    <col collapsed="false" hidden="false" max="24" min="24" style="1" width="22.2793522267206"/>
+    <col collapsed="false" hidden="false" max="25" min="25" style="1" width="117.186234817814"/>
+    <col collapsed="false" hidden="false" max="26" min="26" style="1" width="51.7368421052632"/>
+    <col collapsed="false" hidden="false" max="27" min="27" style="1" width="19.7085020242915"/>
+    <col collapsed="false" hidden="false" max="28" min="28" style="1" width="25.0647773279352"/>
+    <col collapsed="false" hidden="false" max="29" min="29" style="1" width="25.4939271255061"/>
+    <col collapsed="false" hidden="false" max="30" min="30" style="1" width="15.5303643724696"/>
     <col collapsed="false" hidden="false" max="31" min="31" style="1" width="13.6032388663968"/>
-    <col collapsed="false" hidden="false" max="32" min="32" style="1" width="15.8542510121457"/>
+    <col collapsed="false" hidden="false" max="32" min="32" style="1" width="15.9595141700405"/>
     <col collapsed="false" hidden="false" max="33" min="33" style="1" width="13.9271255060729"/>
-    <col collapsed="false" hidden="false" max="34" min="34" style="1" width="12.4251012145749"/>
-    <col collapsed="false" hidden="false" max="35" min="35" style="1" width="12.9595141700405"/>
-    <col collapsed="false" hidden="false" max="36" min="36" style="1" width="59.4493927125506"/>
-    <col collapsed="false" hidden="false" max="37" min="37" style="1" width="25.3886639676113"/>
-    <col collapsed="false" hidden="false" max="38" min="38" style="1" width="20.246963562753"/>
-    <col collapsed="false" hidden="false" max="39" min="39" style="1" width="21.3157894736842"/>
+    <col collapsed="false" hidden="false" max="34" min="34" style="1" width="12.5344129554656"/>
+    <col collapsed="false" hidden="false" max="35" min="35" style="1" width="13.0688259109312"/>
+    <col collapsed="false" hidden="false" max="36" min="36" style="1" width="59.9878542510121"/>
+    <col collapsed="false" hidden="false" max="37" min="37" style="1" width="25.4939271255061"/>
+    <col collapsed="false" hidden="false" max="38" min="38" style="1" width="20.3522267206478"/>
+    <col collapsed="false" hidden="false" max="39" min="39" style="1" width="21.5303643724696"/>
     <col collapsed="false" hidden="false" max="40" min="40" style="1" width="7.60728744939271"/>
     <col collapsed="false" hidden="false" max="41" min="41" style="1" width="8.67611336032389"/>
     <col collapsed="false" hidden="false" max="42" min="42" style="1" width="10.6032388663968"/>
@@ -16594,7 +16592,7 @@
       <c r="X167" s="11"/>
       <c r="Y167" s="11"/>
       <c r="Z167" s="11" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="AA167" s="11"/>
       <c r="AB167" s="14"/>
@@ -16638,23 +16636,23 @@
         <v>44</v>
       </c>
       <c r="D168" s="11" t="s">
+        <v>545</v>
+      </c>
+      <c r="E168" s="30" t="s">
         <v>546</v>
-      </c>
-      <c r="E168" s="30" t="s">
-        <v>547</v>
       </c>
       <c r="F168" s="30"/>
       <c r="G168" s="30" t="s">
+        <v>547</v>
+      </c>
+      <c r="H168" s="30" t="s">
         <v>548</v>
       </c>
-      <c r="H168" s="30" t="s">
+      <c r="I168" s="10" t="s">
         <v>549</v>
       </c>
-      <c r="I168" s="10" t="s">
+      <c r="J168" s="10" t="s">
         <v>550</v>
-      </c>
-      <c r="J168" s="10" t="s">
-        <v>551</v>
       </c>
       <c r="K168" s="13"/>
       <c r="L168" s="13"/>
@@ -16666,7 +16664,7 @@
       <c r="R168" s="11"/>
       <c r="S168" s="11"/>
       <c r="T168" s="11" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="U168" s="11"/>
       <c r="V168" s="11"/>
@@ -16708,23 +16706,23 @@
         <v>44</v>
       </c>
       <c r="D169" s="11" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="E169" s="10" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="F169" s="10"/>
       <c r="G169" s="10" t="s">
+        <v>553</v>
+      </c>
+      <c r="H169" s="31" t="s">
         <v>554</v>
       </c>
-      <c r="H169" s="31" t="s">
-        <v>555</v>
-      </c>
       <c r="I169" s="10" t="s">
+        <v>549</v>
+      </c>
+      <c r="J169" s="10" t="s">
         <v>550</v>
-      </c>
-      <c r="J169" s="10" t="s">
-        <v>551</v>
       </c>
       <c r="K169" s="13"/>
       <c r="L169" s="13"/>
@@ -16736,7 +16734,7 @@
       <c r="R169" s="11"/>
       <c r="S169" s="11"/>
       <c r="T169" s="11" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="U169" s="11"/>
       <c r="V169" s="11"/>
@@ -16762,7 +16760,7 @@
         <v>154</v>
       </c>
       <c r="AP169" s="17" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="AQ169" s="14"/>
       <c r="AMJ169" s="0"/>
@@ -16778,39 +16776,39 @@
         <v>44</v>
       </c>
       <c r="D170" s="11" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="E170" s="30" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="F170" s="30"/>
       <c r="G170" s="30" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="H170" s="30" t="s">
         <v>528</v>
       </c>
       <c r="I170" s="10" t="s">
+        <v>558</v>
+      </c>
+      <c r="J170" s="10" t="s">
         <v>559</v>
-      </c>
-      <c r="J170" s="10" t="s">
-        <v>560</v>
       </c>
       <c r="K170" s="13"/>
       <c r="L170" s="13"/>
       <c r="M170" s="13"/>
       <c r="N170" s="10" t="s">
+        <v>560</v>
+      </c>
+      <c r="O170" s="33" t="s">
         <v>561</v>
-      </c>
-      <c r="O170" s="33" t="s">
-        <v>562</v>
       </c>
       <c r="P170" s="11"/>
       <c r="Q170" s="11"/>
       <c r="R170" s="11"/>
       <c r="S170" s="11"/>
       <c r="T170" s="11" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="U170" s="11"/>
       <c r="V170" s="11"/>
@@ -16852,39 +16850,39 @@
         <v>44</v>
       </c>
       <c r="D171" s="11" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="E171" s="30" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="F171" s="30"/>
       <c r="G171" s="30" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="H171" s="30" t="s">
         <v>528</v>
       </c>
       <c r="I171" s="10" t="s">
+        <v>558</v>
+      </c>
+      <c r="J171" s="10" t="s">
         <v>559</v>
-      </c>
-      <c r="J171" s="10" t="s">
-        <v>560</v>
       </c>
       <c r="K171" s="13"/>
       <c r="L171" s="13"/>
       <c r="M171" s="13"/>
       <c r="N171" s="10" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="O171" s="33" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="P171" s="11"/>
       <c r="Q171" s="11"/>
       <c r="R171" s="11"/>
       <c r="S171" s="11"/>
       <c r="T171" s="11" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="U171" s="11"/>
       <c r="V171" s="11"/>
@@ -16926,39 +16924,39 @@
         <v>44</v>
       </c>
       <c r="D172" s="11" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="E172" s="30" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="F172" s="30"/>
       <c r="G172" s="30" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="H172" s="30" t="s">
         <v>528</v>
       </c>
       <c r="I172" s="10" t="s">
+        <v>558</v>
+      </c>
+      <c r="J172" s="10" t="s">
         <v>559</v>
-      </c>
-      <c r="J172" s="10" t="s">
-        <v>560</v>
       </c>
       <c r="K172" s="13"/>
       <c r="L172" s="13"/>
       <c r="M172" s="13"/>
       <c r="N172" s="10" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="O172" s="33" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="P172" s="11"/>
       <c r="Q172" s="11"/>
       <c r="R172" s="11"/>
       <c r="S172" s="11"/>
       <c r="T172" s="11" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="U172" s="11"/>
       <c r="V172" s="11"/>
@@ -17000,39 +16998,39 @@
         <v>44</v>
       </c>
       <c r="D173" s="11" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="E173" s="30" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="F173" s="30"/>
       <c r="G173" s="30" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="H173" s="30" t="s">
         <v>528</v>
       </c>
       <c r="I173" s="10" t="s">
+        <v>558</v>
+      </c>
+      <c r="J173" s="10" t="s">
         <v>559</v>
-      </c>
-      <c r="J173" s="10" t="s">
-        <v>560</v>
       </c>
       <c r="K173" s="13"/>
       <c r="L173" s="13"/>
       <c r="M173" s="13"/>
       <c r="N173" s="10" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="O173" s="33" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="P173" s="11"/>
       <c r="Q173" s="11"/>
       <c r="R173" s="11"/>
       <c r="S173" s="11"/>
       <c r="T173" s="11" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="U173" s="11"/>
       <c r="V173" s="11"/>
@@ -17074,23 +17072,23 @@
         <v>44</v>
       </c>
       <c r="D174" s="11" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="E174" s="30" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="F174" s="30"/>
       <c r="G174" s="30" t="s">
+        <v>566</v>
+      </c>
+      <c r="H174" s="30" t="s">
         <v>567</v>
       </c>
-      <c r="H174" s="30" t="s">
+      <c r="I174" s="10" t="s">
         <v>568</v>
       </c>
-      <c r="I174" s="10" t="s">
+      <c r="J174" s="10" t="s">
         <v>569</v>
-      </c>
-      <c r="J174" s="10" t="s">
-        <v>570</v>
       </c>
       <c r="K174" s="13"/>
       <c r="L174" s="13"/>
@@ -17102,7 +17100,7 @@
       <c r="R174" s="11"/>
       <c r="S174" s="11"/>
       <c r="T174" s="11" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="U174" s="11"/>
       <c r="V174" s="11"/>
@@ -17128,7 +17126,7 @@
         <v>159</v>
       </c>
       <c r="AP174" s="17" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="AQ174" s="14"/>
       <c r="AMJ174" s="0"/>
@@ -17144,23 +17142,23 @@
         <v>44</v>
       </c>
       <c r="D175" s="11" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="E175" s="30" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="F175" s="30"/>
       <c r="G175" s="30" t="s">
+        <v>572</v>
+      </c>
+      <c r="H175" s="30" t="s">
         <v>573</v>
       </c>
-      <c r="H175" s="30" t="s">
+      <c r="I175" s="10" t="s">
         <v>574</v>
       </c>
-      <c r="I175" s="10" t="s">
-        <v>575</v>
-      </c>
       <c r="J175" s="10" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="K175" s="13"/>
       <c r="L175" s="13"/>
@@ -17172,7 +17170,7 @@
       <c r="R175" s="11"/>
       <c r="S175" s="11"/>
       <c r="T175" s="11" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="U175" s="11"/>
       <c r="V175" s="11"/>
@@ -17214,37 +17212,37 @@
         <v>44</v>
       </c>
       <c r="D176" s="11" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="E176" s="30" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="F176" s="30"/>
       <c r="G176" s="30" t="s">
+        <v>576</v>
+      </c>
+      <c r="H176" s="30" t="s">
         <v>577</v>
       </c>
-      <c r="H176" s="30" t="s">
+      <c r="I176" s="10" t="s">
         <v>578</v>
       </c>
-      <c r="I176" s="10" t="s">
-        <v>579</v>
-      </c>
       <c r="J176" s="10" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="K176" s="13"/>
       <c r="L176" s="13"/>
       <c r="M176" s="13"/>
       <c r="N176" s="10"/>
       <c r="O176" s="10" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="P176" s="11"/>
       <c r="Q176" s="11"/>
       <c r="R176" s="11"/>
       <c r="S176" s="11"/>
       <c r="T176" s="11" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="U176" s="11"/>
       <c r="V176" s="11"/>
@@ -17286,23 +17284,23 @@
         <v>44</v>
       </c>
       <c r="D177" s="11" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="E177" s="30" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="F177" s="30"/>
       <c r="G177" s="30" t="s">
+        <v>582</v>
+      </c>
+      <c r="H177" s="30" t="s">
         <v>583</v>
       </c>
-      <c r="H177" s="30" t="s">
+      <c r="I177" s="10" t="s">
         <v>584</v>
       </c>
-      <c r="I177" s="10" t="s">
-        <v>585</v>
-      </c>
       <c r="J177" s="10" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="K177" s="13"/>
       <c r="L177" s="13"/>
@@ -17316,14 +17314,14 @@
       <c r="R177" s="11"/>
       <c r="S177" s="11"/>
       <c r="T177" s="11" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="U177" s="11"/>
       <c r="V177" s="11"/>
       <c r="W177" s="11"/>
       <c r="X177" s="11"/>
       <c r="Y177" s="36" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="Z177" s="11"/>
       <c r="AA177" s="11"/>
@@ -17358,39 +17356,39 @@
         <v>44</v>
       </c>
       <c r="D178" s="11" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="E178" s="30" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="F178" s="30"/>
       <c r="G178" s="30" t="s">
+        <v>587</v>
+      </c>
+      <c r="H178" s="30" t="s">
         <v>588</v>
       </c>
-      <c r="H178" s="30" t="s">
-        <v>589</v>
-      </c>
       <c r="I178" s="10" t="s">
+        <v>558</v>
+      </c>
+      <c r="J178" s="10" t="s">
         <v>559</v>
-      </c>
-      <c r="J178" s="10" t="s">
-        <v>560</v>
       </c>
       <c r="K178" s="13"/>
       <c r="L178" s="13"/>
       <c r="M178" s="13"/>
       <c r="N178" s="10" t="s">
+        <v>589</v>
+      </c>
+      <c r="O178" s="16" t="s">
         <v>590</v>
-      </c>
-      <c r="O178" s="16" t="s">
-        <v>591</v>
       </c>
       <c r="P178" s="11"/>
       <c r="Q178" s="11"/>
       <c r="R178" s="11"/>
       <c r="S178" s="11"/>
       <c r="T178" s="11" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="U178" s="11"/>
       <c r="V178" s="11"/>
@@ -17432,39 +17430,39 @@
         <v>44</v>
       </c>
       <c r="D179" s="11" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="E179" s="30" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="F179" s="30"/>
       <c r="G179" s="30" t="s">
+        <v>587</v>
+      </c>
+      <c r="H179" s="30" t="s">
         <v>588</v>
       </c>
-      <c r="H179" s="30" t="s">
-        <v>589</v>
-      </c>
       <c r="I179" s="10" t="s">
+        <v>558</v>
+      </c>
+      <c r="J179" s="10" t="s">
         <v>559</v>
-      </c>
-      <c r="J179" s="10" t="s">
-        <v>560</v>
       </c>
       <c r="K179" s="13"/>
       <c r="L179" s="13"/>
       <c r="M179" s="13"/>
       <c r="N179" s="10" t="s">
+        <v>589</v>
+      </c>
+      <c r="O179" s="16" t="s">
         <v>590</v>
-      </c>
-      <c r="O179" s="16" t="s">
-        <v>591</v>
       </c>
       <c r="P179" s="11"/>
       <c r="Q179" s="11"/>
       <c r="R179" s="11"/>
       <c r="S179" s="11"/>
       <c r="T179" s="11" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="U179" s="11"/>
       <c r="V179" s="11"/>
@@ -17506,39 +17504,39 @@
         <v>44</v>
       </c>
       <c r="D180" s="11" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="E180" s="30" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="F180" s="30"/>
       <c r="G180" s="30" t="s">
+        <v>587</v>
+      </c>
+      <c r="H180" s="30" t="s">
         <v>588</v>
       </c>
-      <c r="H180" s="30" t="s">
-        <v>589</v>
-      </c>
       <c r="I180" s="10" t="s">
+        <v>558</v>
+      </c>
+      <c r="J180" s="10" t="s">
         <v>559</v>
-      </c>
-      <c r="J180" s="10" t="s">
-        <v>560</v>
       </c>
       <c r="K180" s="13"/>
       <c r="L180" s="13"/>
       <c r="M180" s="13"/>
       <c r="N180" s="10" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="O180" s="37" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="P180" s="11"/>
       <c r="Q180" s="11"/>
       <c r="R180" s="11"/>
       <c r="S180" s="11"/>
       <c r="T180" s="11" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="U180" s="11"/>
       <c r="V180" s="11"/>
@@ -17580,39 +17578,39 @@
         <v>44</v>
       </c>
       <c r="D181" s="11" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="E181" s="30" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="F181" s="30"/>
       <c r="G181" s="30" t="s">
+        <v>587</v>
+      </c>
+      <c r="H181" s="30" t="s">
         <v>588</v>
       </c>
-      <c r="H181" s="30" t="s">
-        <v>589</v>
-      </c>
       <c r="I181" s="10" t="s">
+        <v>558</v>
+      </c>
+      <c r="J181" s="10" t="s">
         <v>559</v>
-      </c>
-      <c r="J181" s="10" t="s">
-        <v>560</v>
       </c>
       <c r="K181" s="13"/>
       <c r="L181" s="13"/>
       <c r="M181" s="13"/>
       <c r="N181" s="10" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="O181" s="37" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="P181" s="11"/>
       <c r="Q181" s="11"/>
       <c r="R181" s="11"/>
       <c r="S181" s="11"/>
       <c r="T181" s="11" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="U181" s="11"/>
       <c r="V181" s="11"/>
@@ -17638,7 +17636,7 @@
         <v>166</v>
       </c>
       <c r="AP181" s="38" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="AQ181" s="14"/>
       <c r="AMJ181" s="0"/>
@@ -17654,21 +17652,21 @@
         <v>44</v>
       </c>
       <c r="D182" s="39" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="E182" s="40"/>
       <c r="F182" s="30"/>
       <c r="G182" s="40" t="s">
+        <v>594</v>
+      </c>
+      <c r="H182" s="40" t="s">
         <v>595</v>
       </c>
-      <c r="H182" s="40" t="s">
-        <v>596</v>
-      </c>
       <c r="I182" s="39" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="J182" s="39" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="K182" s="41"/>
       <c r="L182" s="41"/>
@@ -17680,7 +17678,7 @@
       <c r="R182" s="39"/>
       <c r="S182" s="39"/>
       <c r="T182" s="39" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="U182" s="39"/>
       <c r="V182" s="39"/>

</xml_diff>

<commit_message>
PROS-9088 - CCRU - update KPIs POS
</commit_message>
<xml_diff>
--- a/Projects/CCRU/Data/KPIs_2019/PoS 2019 - MT Conv Big - REG.xlsx
+++ b/Projects/CCRU/Data/KPIs_2019/PoS 2019 - MT Conv Big - REG.xlsx
@@ -17,6 +17,7 @@
     <definedName function="false" hidden="false" localSheetId="0" name="_FilterDatabase_0_0_0" vbProcedure="false">CONV_BIG_REG!$A$1:$AQ$180</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_FilterDatabase_0_0_0_0" vbProcedure="false">CONV_BIG_REG!$A$1:$AQ$180</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">CONV_BIG_REG!$A$1:$AQ$180</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0" vbProcedure="false">CONV_BIG_REG!$A$1:$AQ$180</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -1672,7 +1673,7 @@
     <t xml:space="preserve">BRAND</t>
   </si>
   <si>
-    <t xml:space="preserve">1 door cooler</t>
+    <t xml:space="preserve">1 door cooler - Modern Trade</t>
   </si>
   <si>
     <t xml:space="preserve">Min 30% Coca-Cola</t>
@@ -1681,7 +1682,7 @@
     <t xml:space="preserve">Холодильники: Мерч. Стандарты. Мин 30% кока-кола</t>
   </si>
   <si>
-    <t xml:space="preserve">2 door cooler, Open Front, Cash Cooler, Cash Cooler (Open Top)</t>
+    <t xml:space="preserve">Company Coolers: 1st Cash Cooler, 2 door cooler - Modern Trade, Open Front - Modern Trade, Cash Cooler (Open Top) - Modern Trade, Coolers - Counter top, 1.5 door cooler</t>
   </si>
   <si>
     <t xml:space="preserve">Cooler: Merch Priorty STD Fuze and Coca-Cola shelf 2-3 </t>
@@ -2001,7 +2002,7 @@
     <numFmt numFmtId="171" formatCode="@"/>
     <numFmt numFmtId="172" formatCode="#,##0.0000000"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -2042,6 +2043,13 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
     </font>
   </fonts>
   <fills count="3">
@@ -2115,7 +2123,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="33">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -2200,6 +2208,14 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="165" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -2263,57 +2279,57 @@
   </sheetPr>
   <dimension ref="A1:AQ181"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="J1" colorId="64" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A24" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="J1" activeCellId="0" sqref="J1"/>
-      <selection pane="bottomLeft" activeCell="T37" activeCellId="0" sqref="T37"/>
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="Y1" colorId="64" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1" topLeftCell="A129" activePane="bottomLeft" state="frozen"/>
+      <selection pane="topLeft" activeCell="Y1" activeCellId="0" sqref="Y1"/>
+      <selection pane="bottomLeft" activeCell="Z153" activeCellId="0" sqref="Z153:Z154"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="10.2834008097166"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="11.2631578947368"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="18.2388663967611"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="10.3886639676113"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="11.246963562753"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="18.3157894736842"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="1" width="11.1417004048583"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="15.3036437246964"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="42.7246963562753"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="48.2307692307692"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="66.3481781376518"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="47.8663967611336"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="16.5263157894737"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="9.18218623481781"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="13.4696356275304"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="15.4251012145749"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="43.17004048583"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="48.6315789473684"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="66.9473684210526"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="48.3117408906883"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="16.7125506072875"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="9.21052631578947"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="13.497975708502"/>
     <col collapsed="false" hidden="false" max="13" min="13" style="1" width="13.7125506072874"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="57.417004048583"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="30.9716599190283"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="1" width="19.82995951417"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="1" width="16.1619433198381"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="1" width="9.30364372469636"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="1" width="19.0971659919028"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="57.9514170040486"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="31.2793522267206"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="1" width="19.9230769230769"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="1" width="16.1740890688259"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="1" width="9.31983805668016"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="1" width="19.2834008097166"/>
     <col collapsed="false" hidden="false" max="20" min="20" style="1" width="13.7125506072874"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="1" width="7.09716599190283"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="1" width="14.2024291497976"/>
-    <col collapsed="false" hidden="false" max="23" min="23" style="1" width="82.2672064777328"/>
-    <col collapsed="false" hidden="false" max="24" min="24" style="1" width="22.7651821862348"/>
-    <col collapsed="false" hidden="false" max="25" min="25" style="1" width="120.093117408907"/>
-    <col collapsed="false" hidden="false" max="26" min="26" style="1" width="53.0080971659919"/>
-    <col collapsed="false" hidden="false" max="27" min="27" style="1" width="20.1943319838057"/>
-    <col collapsed="false" hidden="false" max="28" min="28" style="1" width="25.587044534413"/>
-    <col collapsed="false" hidden="false" max="29" min="29" style="1" width="25.9514170040486"/>
-    <col collapsed="false" hidden="false" max="30" min="30" style="1" width="15.919028340081"/>
-    <col collapsed="false" hidden="false" max="31" min="31" style="1" width="13.9554655870445"/>
-    <col collapsed="false" hidden="false" max="32" min="32" style="1" width="16.4048582995951"/>
-    <col collapsed="false" hidden="false" max="33" min="33" style="1" width="14.2024291497976"/>
-    <col collapsed="false" hidden="false" max="34" min="34" style="1" width="12.8542510121458"/>
-    <col collapsed="false" hidden="false" max="35" min="35" style="1" width="13.2267206477733"/>
-    <col collapsed="false" hidden="false" max="36" min="36" style="1" width="61.4574898785425"/>
-    <col collapsed="false" hidden="false" max="37" min="37" style="1" width="25.9514170040486"/>
-    <col collapsed="false" hidden="false" max="38" min="38" style="1" width="20.6882591093117"/>
-    <col collapsed="false" hidden="false" max="39" min="39" style="1" width="22.1578947368421"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="1" width="7.17813765182186"/>
+    <col collapsed="false" hidden="false" max="22" min="22" style="1" width="14.3522267206478"/>
+    <col collapsed="false" hidden="false" max="23" min="23" style="1" width="82.9109311740891"/>
+    <col collapsed="false" hidden="false" max="24" min="24" style="1" width="22.9230769230769"/>
+    <col collapsed="false" hidden="false" max="25" min="25" style="1" width="121.14979757085"/>
+    <col collapsed="false" hidden="false" max="26" min="26" style="1" width="53.4534412955466"/>
+    <col collapsed="false" hidden="false" max="27" min="27" style="1" width="20.3522267206478"/>
+    <col collapsed="false" hidden="false" max="28" min="28" style="1" width="25.7085020242915"/>
+    <col collapsed="false" hidden="false" max="29" min="29" style="1" width="26.1376518218623"/>
+    <col collapsed="false" hidden="false" max="30" min="30" style="1" width="15.9595141700405"/>
+    <col collapsed="false" hidden="false" max="31" min="31" style="1" width="14.0323886639676"/>
+    <col collapsed="false" hidden="false" max="32" min="32" style="1" width="16.497975708502"/>
+    <col collapsed="false" hidden="false" max="33" min="33" style="1" width="14.3522267206478"/>
+    <col collapsed="false" hidden="false" max="34" min="34" style="1" width="12.9595141700405"/>
+    <col collapsed="false" hidden="false" max="35" min="35" style="1" width="13.2834008097166"/>
+    <col collapsed="false" hidden="false" max="36" min="36" style="1" width="61.914979757085"/>
+    <col collapsed="false" hidden="false" max="37" min="37" style="1" width="26.1376518218623"/>
+    <col collapsed="false" hidden="false" max="38" min="38" style="1" width="20.7813765182186"/>
+    <col collapsed="false" hidden="false" max="39" min="39" style="1" width="22.2793522267206"/>
     <col collapsed="false" hidden="false" max="40" min="40" style="1" width="7.71255060728745"/>
-    <col collapsed="false" hidden="false" max="41" min="41" style="1" width="8.93522267206478"/>
-    <col collapsed="false" hidden="false" max="42" min="42" style="1" width="10.7773279352227"/>
-    <col collapsed="false" hidden="false" max="1025" min="43" style="1" width="9.30364372469636"/>
+    <col collapsed="false" hidden="false" max="41" min="41" style="1" width="8.89068825910931"/>
+    <col collapsed="false" hidden="false" max="42" min="42" style="1" width="10.8178137651822"/>
+    <col collapsed="false" hidden="false" max="1025" min="43" style="1" width="9.31983805668016"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -15142,7 +15158,7 @@
       <c r="Y153" s="9" t="s">
         <v>472</v>
       </c>
-      <c r="Z153" s="9" t="s">
+      <c r="Z153" s="21" t="s">
         <v>500</v>
       </c>
       <c r="AA153" s="9"/>
@@ -15229,7 +15245,7 @@
       <c r="Y154" s="9" t="s">
         <v>472</v>
       </c>
-      <c r="Z154" s="9" t="s">
+      <c r="Z154" s="22" t="s">
         <v>503</v>
       </c>
       <c r="AA154" s="9"/>
@@ -15694,10 +15710,10 @@
       <c r="D160" s="9" t="s">
         <v>341</v>
       </c>
-      <c r="E160" s="21" t="s">
+      <c r="E160" s="23" t="s">
         <v>394</v>
       </c>
-      <c r="F160" s="21"/>
+      <c r="F160" s="23"/>
       <c r="G160" s="9" t="s">
         <v>519</v>
       </c>
@@ -15713,7 +15729,7 @@
       </c>
       <c r="L160" s="11"/>
       <c r="M160" s="11"/>
-      <c r="N160" s="22"/>
+      <c r="N160" s="24"/>
       <c r="O160" s="9"/>
       <c r="P160" s="9"/>
       <c r="Q160" s="9"/>
@@ -15725,7 +15741,7 @@
       <c r="U160" s="9"/>
       <c r="V160" s="9"/>
       <c r="W160" s="9"/>
-      <c r="X160" s="22"/>
+      <c r="X160" s="24"/>
       <c r="Y160" s="8" t="s">
         <v>519</v>
       </c>
@@ -15775,10 +15791,10 @@
       <c r="D161" s="9" t="s">
         <v>341</v>
       </c>
-      <c r="E161" s="21" t="s">
+      <c r="E161" s="23" t="s">
         <v>394</v>
       </c>
-      <c r="F161" s="21"/>
+      <c r="F161" s="23"/>
       <c r="G161" s="9" t="s">
         <v>521</v>
       </c>
@@ -15814,7 +15830,7 @@
       <c r="U161" s="9"/>
       <c r="V161" s="9"/>
       <c r="W161" s="9"/>
-      <c r="X161" s="22"/>
+      <c r="X161" s="24"/>
       <c r="Y161" s="8" t="s">
         <v>519</v>
       </c>
@@ -15860,8 +15876,8 @@
         <v>44</v>
       </c>
       <c r="D162" s="9"/>
-      <c r="E162" s="21"/>
-      <c r="F162" s="21"/>
+      <c r="E162" s="23"/>
+      <c r="F162" s="23"/>
       <c r="G162" s="9" t="s">
         <v>526</v>
       </c>
@@ -16267,7 +16283,7 @@
       <c r="L167" s="11"/>
       <c r="M167" s="11"/>
       <c r="N167" s="9"/>
-      <c r="O167" s="23" t="s">
+      <c r="O167" s="25" t="s">
         <v>544</v>
       </c>
       <c r="P167" s="9"/>
@@ -16330,14 +16346,14 @@
       <c r="D168" s="9" t="s">
         <v>545</v>
       </c>
-      <c r="E168" s="24" t="s">
+      <c r="E168" s="26" t="s">
         <v>546</v>
       </c>
-      <c r="F168" s="24"/>
-      <c r="G168" s="24" t="s">
+      <c r="F168" s="26"/>
+      <c r="G168" s="26" t="s">
         <v>547</v>
       </c>
-      <c r="H168" s="24" t="s">
+      <c r="H168" s="26" t="s">
         <v>548</v>
       </c>
       <c r="I168" s="8" t="s">
@@ -16406,7 +16422,7 @@
       <c r="G169" s="8" t="s">
         <v>553</v>
       </c>
-      <c r="H169" s="25" t="s">
+      <c r="H169" s="27" t="s">
         <v>554</v>
       </c>
       <c r="I169" s="8" t="s">
@@ -16419,7 +16435,7 @@
       <c r="L169" s="11"/>
       <c r="M169" s="11"/>
       <c r="N169" s="8"/>
-      <c r="O169" s="26"/>
+      <c r="O169" s="28"/>
       <c r="P169" s="9"/>
       <c r="Q169" s="9"/>
       <c r="R169" s="9"/>
@@ -16468,14 +16484,14 @@
       <c r="D170" s="9" t="s">
         <v>545</v>
       </c>
-      <c r="E170" s="24" t="s">
+      <c r="E170" s="26" t="s">
         <v>556</v>
       </c>
-      <c r="F170" s="24"/>
-      <c r="G170" s="24" t="s">
+      <c r="F170" s="26"/>
+      <c r="G170" s="26" t="s">
         <v>557</v>
       </c>
-      <c r="H170" s="24" t="s">
+      <c r="H170" s="26" t="s">
         <v>528</v>
       </c>
       <c r="I170" s="8" t="s">
@@ -16541,14 +16557,14 @@
       <c r="D171" s="9" t="s">
         <v>545</v>
       </c>
-      <c r="E171" s="24" t="s">
+      <c r="E171" s="26" t="s">
         <v>556</v>
       </c>
-      <c r="F171" s="24"/>
-      <c r="G171" s="24" t="s">
+      <c r="F171" s="26"/>
+      <c r="G171" s="26" t="s">
         <v>557</v>
       </c>
-      <c r="H171" s="24" t="s">
+      <c r="H171" s="26" t="s">
         <v>528</v>
       </c>
       <c r="I171" s="8" t="s">
@@ -16614,14 +16630,14 @@
       <c r="D172" s="9" t="s">
         <v>545</v>
       </c>
-      <c r="E172" s="24" t="s">
+      <c r="E172" s="26" t="s">
         <v>556</v>
       </c>
-      <c r="F172" s="24"/>
-      <c r="G172" s="24" t="s">
+      <c r="F172" s="26"/>
+      <c r="G172" s="26" t="s">
         <v>557</v>
       </c>
-      <c r="H172" s="24" t="s">
+      <c r="H172" s="26" t="s">
         <v>528</v>
       </c>
       <c r="I172" s="8" t="s">
@@ -16687,14 +16703,14 @@
       <c r="D173" s="9" t="s">
         <v>545</v>
       </c>
-      <c r="E173" s="24" t="s">
+      <c r="E173" s="26" t="s">
         <v>556</v>
       </c>
-      <c r="F173" s="24"/>
-      <c r="G173" s="24" t="s">
+      <c r="F173" s="26"/>
+      <c r="G173" s="26" t="s">
         <v>557</v>
       </c>
-      <c r="H173" s="24" t="s">
+      <c r="H173" s="26" t="s">
         <v>528</v>
       </c>
       <c r="I173" s="8" t="s">
@@ -16760,14 +16776,14 @@
       <c r="D174" s="9" t="s">
         <v>545</v>
       </c>
-      <c r="E174" s="24" t="s">
+      <c r="E174" s="26" t="s">
         <v>565</v>
       </c>
-      <c r="F174" s="24"/>
-      <c r="G174" s="24" t="s">
+      <c r="F174" s="26"/>
+      <c r="G174" s="26" t="s">
         <v>566</v>
       </c>
-      <c r="H174" s="24" t="s">
+      <c r="H174" s="26" t="s">
         <v>567</v>
       </c>
       <c r="I174" s="8" t="s">
@@ -16780,7 +16796,7 @@
       <c r="L174" s="11"/>
       <c r="M174" s="11"/>
       <c r="N174" s="8"/>
-      <c r="O174" s="27"/>
+      <c r="O174" s="29"/>
       <c r="P174" s="9"/>
       <c r="Q174" s="9"/>
       <c r="R174" s="9"/>
@@ -16829,14 +16845,14 @@
       <c r="D175" s="9" t="s">
         <v>545</v>
       </c>
-      <c r="E175" s="24" t="s">
+      <c r="E175" s="26" t="s">
         <v>571</v>
       </c>
-      <c r="F175" s="24"/>
-      <c r="G175" s="24" t="s">
+      <c r="F175" s="26"/>
+      <c r="G175" s="26" t="s">
         <v>572</v>
       </c>
-      <c r="H175" s="24" t="s">
+      <c r="H175" s="26" t="s">
         <v>573</v>
       </c>
       <c r="I175" s="8" t="s">
@@ -16898,14 +16914,14 @@
       <c r="D176" s="9" t="s">
         <v>545</v>
       </c>
-      <c r="E176" s="24" t="s">
+      <c r="E176" s="26" t="s">
         <v>575</v>
       </c>
-      <c r="F176" s="24"/>
-      <c r="G176" s="24" t="s">
+      <c r="F176" s="26"/>
+      <c r="G176" s="26" t="s">
         <v>576</v>
       </c>
-      <c r="H176" s="24" t="s">
+      <c r="H176" s="26" t="s">
         <v>577</v>
       </c>
       <c r="I176" s="8" t="s">
@@ -16969,14 +16985,14 @@
       <c r="D177" s="9" t="s">
         <v>545</v>
       </c>
-      <c r="E177" s="24" t="s">
+      <c r="E177" s="26" t="s">
         <v>581</v>
       </c>
-      <c r="F177" s="24"/>
-      <c r="G177" s="24" t="s">
+      <c r="F177" s="26"/>
+      <c r="G177" s="26" t="s">
         <v>582</v>
       </c>
-      <c r="H177" s="24" t="s">
+      <c r="H177" s="26" t="s">
         <v>583</v>
       </c>
       <c r="I177" s="8" t="s">
@@ -17040,14 +17056,14 @@
       <c r="D178" s="9" t="s">
         <v>545</v>
       </c>
-      <c r="E178" s="24" t="s">
+      <c r="E178" s="26" t="s">
         <v>586</v>
       </c>
-      <c r="F178" s="24"/>
-      <c r="G178" s="24" t="s">
+      <c r="F178" s="26"/>
+      <c r="G178" s="26" t="s">
         <v>587</v>
       </c>
-      <c r="H178" s="24" t="s">
+      <c r="H178" s="26" t="s">
         <v>588</v>
       </c>
       <c r="I178" s="8" t="s">
@@ -17113,14 +17129,14 @@
       <c r="D179" s="9" t="s">
         <v>545</v>
       </c>
-      <c r="E179" s="24" t="s">
+      <c r="E179" s="26" t="s">
         <v>586</v>
       </c>
-      <c r="F179" s="24"/>
-      <c r="G179" s="24" t="s">
+      <c r="F179" s="26"/>
+      <c r="G179" s="26" t="s">
         <v>587</v>
       </c>
-      <c r="H179" s="24" t="s">
+      <c r="H179" s="26" t="s">
         <v>588</v>
       </c>
       <c r="I179" s="8" t="s">
@@ -17135,7 +17151,7 @@
       <c r="N179" s="8" t="s">
         <v>589</v>
       </c>
-      <c r="O179" s="28" t="s">
+      <c r="O179" s="30" t="s">
         <v>592</v>
       </c>
       <c r="P179" s="9"/>
@@ -17186,14 +17202,14 @@
       <c r="D180" s="9" t="s">
         <v>545</v>
       </c>
-      <c r="E180" s="24" t="s">
+      <c r="E180" s="26" t="s">
         <v>586</v>
       </c>
-      <c r="F180" s="24"/>
-      <c r="G180" s="24" t="s">
+      <c r="F180" s="26"/>
+      <c r="G180" s="26" t="s">
         <v>587</v>
       </c>
-      <c r="H180" s="24" t="s">
+      <c r="H180" s="26" t="s">
         <v>588</v>
       </c>
       <c r="I180" s="8" t="s">
@@ -17208,7 +17224,7 @@
       <c r="N180" s="8" t="s">
         <v>589</v>
       </c>
-      <c r="O180" s="28" t="s">
+      <c r="O180" s="30" t="s">
         <v>593</v>
       </c>
       <c r="P180" s="9"/>
@@ -17259,12 +17275,12 @@
       <c r="D181" s="8" t="s">
         <v>545</v>
       </c>
-      <c r="E181" s="24"/>
-      <c r="F181" s="24"/>
-      <c r="G181" s="24" t="s">
+      <c r="E181" s="26"/>
+      <c r="F181" s="26"/>
+      <c r="G181" s="26" t="s">
         <v>595</v>
       </c>
-      <c r="H181" s="24" t="s">
+      <c r="H181" s="26" t="s">
         <v>596</v>
       </c>
       <c r="I181" s="8" t="s">
@@ -17276,7 +17292,7 @@
       <c r="K181" s="11"/>
       <c r="L181" s="11"/>
       <c r="M181" s="8"/>
-      <c r="N181" s="28"/>
+      <c r="N181" s="30"/>
       <c r="O181" s="8"/>
       <c r="P181" s="8"/>
       <c r="Q181" s="8"/>
@@ -17294,12 +17310,12 @@
       <c r="AA181" s="8"/>
       <c r="AB181" s="8"/>
       <c r="AC181" s="8"/>
-      <c r="AD181" s="29"/>
+      <c r="AD181" s="31"/>
       <c r="AE181" s="8"/>
       <c r="AF181" s="8"/>
       <c r="AG181" s="8"/>
       <c r="AH181" s="8"/>
-      <c r="AI181" s="30"/>
+      <c r="AI181" s="32"/>
       <c r="AJ181" s="8"/>
       <c r="AK181" s="8"/>
       <c r="AL181" s="9"/>

</xml_diff>